<commit_message>
Update README.md. Update copyright
</commit_message>
<xml_diff>
--- a/Module1/44825-graphics-training.xlsx
+++ b/Module1/44825-graphics-training.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\AI-CS - Repo\TP1\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\AI\Module1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CF9B3D-B843-40A0-861B-6300A9A25CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97BC6CF-BA4F-4544-8949-90486290B387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2172" yWindow="2136" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{A25E9922-9FA5-4956-A6CE-2560104ACAF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{A25E9922-9FA5-4956-A6CE-2560104ACAF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha3" sheetId="3" state="hidden" r:id="rId1"/>
@@ -76,16 +76,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,12 +105,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -141,7 +134,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -178,7 +171,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1306,7 +1299,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1526493424"/>
@@ -1365,7 +1358,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="625752128"/>
@@ -1407,7 +1400,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1444,7 +1437,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1458,7 +1451,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1520,7 +1513,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5771,7 +5764,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1851338655"/>
@@ -5830,7 +5823,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2114215007"/>
@@ -5872,7 +5865,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5909,7 +5902,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5923,7 +5916,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5990,7 +5983,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11171,7 +11164,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2028845183"/>
@@ -11230,7 +11223,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2122182367"/>
@@ -11282,7 +11275,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11319,7 +11312,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11333,7 +11326,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -11400,7 +11393,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -17205,7 +17198,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2028845183"/>
@@ -17264,7 +17257,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2122182367"/>
@@ -17316,7 +17309,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -17353,7 +17346,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -19742,7 +19735,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -21201,14 +21194,14 @@
   <dimension ref="A1:E202"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.88671875" customWidth="1"/>
   </cols>
@@ -21220,7 +21213,7 @@
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -21237,7 +21230,7 @@
       <c r="B2" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>0.17</v>
       </c>
       <c r="D2" s="1">
@@ -21254,7 +21247,7 @@
       <c r="B3" s="1">
         <v>0.12</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>0.23</v>
       </c>
       <c r="D3" s="1">
@@ -21271,7 +21264,7 @@
       <c r="B4" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>0.25</v>
       </c>
       <c r="D4" s="1">
@@ -21288,7 +21281,7 @@
       <c r="B5" s="1">
         <v>0.18</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>0.25</v>
       </c>
       <c r="D5" s="1">
@@ -21305,7 +21298,7 @@
       <c r="B6" s="1">
         <v>0.18</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>0.25</v>
       </c>
       <c r="D6" s="1">
@@ -21322,7 +21315,7 @@
       <c r="B7" s="1">
         <v>0.21</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>0.25</v>
       </c>
       <c r="D7" s="1">
@@ -21339,7 +21332,7 @@
       <c r="B8" s="1">
         <v>0.21</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>0.25</v>
       </c>
       <c r="D8" s="1">
@@ -21356,7 +21349,7 @@
       <c r="B9" s="1">
         <v>0.23</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>0.25</v>
       </c>
       <c r="D9" s="1">
@@ -21373,7 +21366,7 @@
       <c r="B10" s="1">
         <v>0.23</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>0.25</v>
       </c>
       <c r="D10" s="1">
@@ -21390,7 +21383,7 @@
       <c r="B11" s="1">
         <v>0.24</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>0.25</v>
       </c>
       <c r="D11" s="1">
@@ -21407,7 +21400,7 @@
       <c r="B12" s="1">
         <v>0.23</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>0.25</v>
       </c>
       <c r="D12" s="1">
@@ -21424,7 +21417,7 @@
       <c r="B13" s="1">
         <v>0.25</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>0.25</v>
       </c>
       <c r="D13" s="1">
@@ -21441,7 +21434,7 @@
       <c r="B14" s="1">
         <v>0.24</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>0.25</v>
       </c>
       <c r="D14" s="1">
@@ -21458,7 +21451,7 @@
       <c r="B15" s="1">
         <v>0.25</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>0.25</v>
       </c>
       <c r="D15" s="1">
@@ -21475,7 +21468,7 @@
       <c r="B16" s="1">
         <v>0.24</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>0.25</v>
       </c>
       <c r="D16" s="1">
@@ -21492,7 +21485,7 @@
       <c r="B17" s="1">
         <v>0.25</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>0.25</v>
       </c>
       <c r="D17" s="1">
@@ -21509,7 +21502,7 @@
       <c r="B18" s="1">
         <v>0.24</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>0.25</v>
       </c>
       <c r="D18" s="1">
@@ -21526,7 +21519,7 @@
       <c r="B19" s="1">
         <v>0.25</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>0.25</v>
       </c>
       <c r="D19" s="1">
@@ -21543,7 +21536,7 @@
       <c r="B20" s="1">
         <v>0.24</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>0.25</v>
       </c>
       <c r="D20" s="1">
@@ -21560,7 +21553,7 @@
       <c r="B21" s="1">
         <v>0.25</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>0.25</v>
       </c>
       <c r="D21" s="1">
@@ -21577,7 +21570,7 @@
       <c r="B22" s="1">
         <v>0.24</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>0.25</v>
       </c>
       <c r="D22" s="1">
@@ -21594,7 +21587,7 @@
       <c r="B23" s="1">
         <v>0.25</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="3">
         <v>0.25</v>
       </c>
       <c r="D23" s="1">
@@ -21611,7 +21604,7 @@
       <c r="B24" s="1">
         <v>0.24</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="3">
         <v>0.25</v>
       </c>
       <c r="D24" s="1">
@@ -21628,7 +21621,7 @@
       <c r="B25" s="1">
         <v>0.25</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="3">
         <v>0.25</v>
       </c>
       <c r="D25" s="1">
@@ -21645,7 +21638,7 @@
       <c r="B26" s="1">
         <v>0.24</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="3">
         <v>0.25</v>
       </c>
       <c r="D26" s="1">
@@ -21662,7 +21655,7 @@
       <c r="B27" s="1">
         <v>0.25</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <v>0.25</v>
       </c>
       <c r="D27" s="1">
@@ -21679,7 +21672,7 @@
       <c r="B28" s="1">
         <v>0.24</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="3">
         <v>0.25</v>
       </c>
       <c r="D28" s="1">
@@ -21696,7 +21689,7 @@
       <c r="B29" s="1">
         <v>0.25</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="3">
         <v>0.25</v>
       </c>
       <c r="D29" s="1">
@@ -21713,7 +21706,7 @@
       <c r="B30" s="1">
         <v>0.24</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="3">
         <v>0.25</v>
       </c>
       <c r="D30" s="1">
@@ -21730,7 +21723,7 @@
       <c r="B31" s="1">
         <v>0.25</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="3">
         <v>0.25</v>
       </c>
       <c r="D31" s="1">
@@ -21747,7 +21740,7 @@
       <c r="B32" s="1">
         <v>0.24</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="3">
         <v>0.25</v>
       </c>
       <c r="D32" s="1">
@@ -21764,7 +21757,7 @@
       <c r="B33" s="1">
         <v>0.25</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="3">
         <v>0.25</v>
       </c>
       <c r="D33" s="1">
@@ -21781,7 +21774,7 @@
       <c r="B34" s="1">
         <v>0.24</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="3">
         <v>0.25</v>
       </c>
       <c r="D34" s="1">
@@ -21798,7 +21791,7 @@
       <c r="B35" s="1">
         <v>0.25</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="3">
         <v>0.25</v>
       </c>
       <c r="D35" s="1">
@@ -21815,7 +21808,7 @@
       <c r="B36" s="1">
         <v>0.24</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="3">
         <v>0.25</v>
       </c>
       <c r="D36" s="1">
@@ -21832,7 +21825,7 @@
       <c r="B37" s="1">
         <v>0.25</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="3">
         <v>0.25</v>
       </c>
       <c r="D37" s="1">
@@ -21849,7 +21842,7 @@
       <c r="B38" s="1">
         <v>0.24</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="3">
         <v>0.25</v>
       </c>
       <c r="D38" s="1">
@@ -21866,7 +21859,7 @@
       <c r="B39" s="1">
         <v>0.25</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="3">
         <v>0.25</v>
       </c>
       <c r="D39" s="1">
@@ -21883,7 +21876,7 @@
       <c r="B40" s="1">
         <v>0.24</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="3">
         <v>0.25</v>
       </c>
       <c r="D40" s="1">
@@ -21900,7 +21893,7 @@
       <c r="B41" s="1">
         <v>0.25</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="3">
         <v>0.25</v>
       </c>
       <c r="D41" s="1">
@@ -21917,7 +21910,7 @@
       <c r="B42" s="1">
         <v>0.24</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="3">
         <v>0.25</v>
       </c>
       <c r="D42" s="1">
@@ -21934,7 +21927,7 @@
       <c r="B43" s="1">
         <v>0.25</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="3">
         <v>0.25</v>
       </c>
       <c r="D43" s="1">
@@ -21951,7 +21944,7 @@
       <c r="B44" s="1">
         <v>0.24</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="3">
         <v>0.25</v>
       </c>
       <c r="D44" s="1">
@@ -21968,7 +21961,7 @@
       <c r="B45" s="1">
         <v>0.25</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="3">
         <v>0.25</v>
       </c>
       <c r="D45" s="1">
@@ -21985,7 +21978,7 @@
       <c r="B46" s="1">
         <v>0.24</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="3">
         <v>0.25</v>
       </c>
       <c r="D46" s="1">
@@ -22002,7 +21995,7 @@
       <c r="B47" s="1">
         <v>0.25</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="3">
         <v>0.25</v>
       </c>
       <c r="D47" s="1">
@@ -22019,7 +22012,7 @@
       <c r="B48" s="1">
         <v>0.24</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="3">
         <v>0.25</v>
       </c>
       <c r="D48" s="1">
@@ -22036,7 +22029,7 @@
       <c r="B49" s="1">
         <v>0.25</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="3">
         <v>0.25</v>
       </c>
       <c r="D49" s="1">
@@ -22051,7 +22044,7 @@
       <c r="B50" s="1">
         <v>0.24</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="3">
         <v>0.25</v>
       </c>
       <c r="D50" s="1">
@@ -22066,7 +22059,7 @@
       <c r="B51" s="1">
         <v>0.25</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="3">
         <v>0.25</v>
       </c>
       <c r="D51" s="1">
@@ -22081,7 +22074,7 @@
       <c r="B52" s="1">
         <v>0.24</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="3">
         <v>0.25</v>
       </c>
       <c r="D52" s="1">
@@ -22096,7 +22089,7 @@
       <c r="B53" s="1">
         <v>0.25</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="3">
         <v>0.24</v>
       </c>
       <c r="D53" s="1">
@@ -22111,7 +22104,7 @@
       <c r="B54" s="1">
         <v>0.24</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="3">
         <v>0.24</v>
       </c>
       <c r="D54" s="1">
@@ -22126,7 +22119,7 @@
       <c r="B55" s="1">
         <v>0.25</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="3">
         <v>0.24</v>
       </c>
       <c r="D55" s="1">
@@ -22141,7 +22134,7 @@
       <c r="B56" s="1">
         <v>0.24</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="3">
         <v>0.24</v>
       </c>
       <c r="D56" s="1">
@@ -22156,7 +22149,7 @@
       <c r="B57" s="1">
         <v>0.25</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="3">
         <v>0.24</v>
       </c>
       <c r="D57" s="1">
@@ -22171,7 +22164,7 @@
       <c r="B58" s="1">
         <v>0.24</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="3">
         <v>0.24</v>
       </c>
       <c r="D58" s="1">
@@ -22186,7 +22179,7 @@
       <c r="B59" s="1">
         <v>0.25</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="3">
         <v>0.24</v>
       </c>
       <c r="D59" s="1">
@@ -22201,7 +22194,7 @@
       <c r="B60" s="1">
         <v>0.24</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="3">
         <v>0.24</v>
       </c>
       <c r="D60" s="1">
@@ -22216,7 +22209,7 @@
       <c r="B61" s="1">
         <v>0.25</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="3">
         <v>0.24</v>
       </c>
       <c r="D61" s="1">
@@ -22231,7 +22224,7 @@
       <c r="B62" s="1">
         <v>0.24</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="3">
         <v>0.24</v>
       </c>
       <c r="D62" s="1">
@@ -22246,7 +22239,7 @@
       <c r="B63" s="1">
         <v>0.25</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="3">
         <v>0.24</v>
       </c>
       <c r="D63" s="1">
@@ -22261,7 +22254,7 @@
       <c r="B64" s="1">
         <v>0.24</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="3">
         <v>0.24</v>
       </c>
       <c r="D64" s="1">
@@ -22276,7 +22269,7 @@
       <c r="B65" s="1">
         <v>0.25</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="3">
         <v>0.24</v>
       </c>
       <c r="D65" s="1">
@@ -22291,7 +22284,7 @@
       <c r="B66" s="1">
         <v>0.24</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="3">
         <v>0.24</v>
       </c>
       <c r="D66" s="1">
@@ -22306,7 +22299,7 @@
       <c r="B67" s="1">
         <v>0.25</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="3">
         <v>0.24</v>
       </c>
       <c r="D67" s="1">
@@ -22321,7 +22314,7 @@
       <c r="B68" s="1">
         <v>0.24</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="3">
         <v>0.24</v>
       </c>
       <c r="D68" s="1">
@@ -22336,7 +22329,7 @@
       <c r="B69" s="1">
         <v>0.25</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="3">
         <v>0.24</v>
       </c>
       <c r="D69" s="1">
@@ -22351,7 +22344,7 @@
       <c r="B70" s="1">
         <v>0.24</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="3">
         <v>0.24</v>
       </c>
       <c r="D70" s="1">
@@ -22366,7 +22359,7 @@
       <c r="B71" s="1">
         <v>0.25</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="3">
         <v>0.24</v>
       </c>
       <c r="D71" s="1">
@@ -22381,7 +22374,7 @@
       <c r="B72" s="1">
         <v>0.24</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="3">
         <v>0.23</v>
       </c>
       <c r="D72" s="1">
@@ -22396,7 +22389,7 @@
       <c r="B73" s="1">
         <v>0.25</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="3">
         <v>0.23</v>
       </c>
       <c r="D73" s="1">
@@ -22411,7 +22404,7 @@
       <c r="B74" s="1">
         <v>0.24</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="3">
         <v>0.23</v>
       </c>
       <c r="D74" s="1">
@@ -22426,7 +22419,7 @@
       <c r="B75" s="1">
         <v>0.25</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="3">
         <v>0.23</v>
       </c>
       <c r="D75" s="1">
@@ -22441,7 +22434,7 @@
       <c r="B76" s="1">
         <v>0.24</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="3">
         <v>0.23</v>
       </c>
       <c r="D76" s="1">
@@ -22456,7 +22449,7 @@
       <c r="B77" s="1">
         <v>0.25</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="3">
         <v>0.23</v>
       </c>
       <c r="D77" s="1">
@@ -22471,7 +22464,7 @@
       <c r="B78" s="1">
         <v>0.24</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="3">
         <v>0.23</v>
       </c>
       <c r="D78" s="1">
@@ -22486,7 +22479,7 @@
       <c r="B79" s="1">
         <v>0.25</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="3">
         <v>0.23</v>
       </c>
       <c r="D79" s="1">
@@ -22501,7 +22494,7 @@
       <c r="B80" s="1">
         <v>0.24</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="3">
         <v>0.23</v>
       </c>
       <c r="D80" s="1">
@@ -22516,7 +22509,7 @@
       <c r="B81" s="1">
         <v>0.25</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="3">
         <v>0.23</v>
       </c>
       <c r="D81" s="1">
@@ -22531,7 +22524,7 @@
       <c r="B82" s="1">
         <v>0.24</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="3">
         <v>0.22</v>
       </c>
       <c r="D82" s="1">
@@ -22546,7 +22539,7 @@
       <c r="B83" s="1">
         <v>0.25</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="3">
         <v>0.23</v>
       </c>
       <c r="D83" s="1">
@@ -22561,7 +22554,7 @@
       <c r="B84" s="1">
         <v>0.24</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84" s="3">
         <v>0.22</v>
       </c>
       <c r="D84" s="1">
@@ -22576,7 +22569,7 @@
       <c r="B85" s="1">
         <v>0.25</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85" s="3">
         <v>0.22</v>
       </c>
       <c r="D85" s="1">
@@ -22591,7 +22584,7 @@
       <c r="B86" s="1">
         <v>0.24</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="3">
         <v>0.22</v>
       </c>
       <c r="D86" s="1">
@@ -22606,7 +22599,7 @@
       <c r="B87" s="1">
         <v>0.25</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="3">
         <v>0.22</v>
       </c>
       <c r="D87" s="1">
@@ -22621,7 +22614,7 @@
       <c r="B88" s="1">
         <v>0.24</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88" s="3">
         <v>0.22</v>
       </c>
       <c r="D88" s="1">
@@ -22636,7 +22629,7 @@
       <c r="B89" s="1">
         <v>0.25</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="3">
         <v>0.22</v>
       </c>
       <c r="D89" s="1">
@@ -22651,7 +22644,7 @@
       <c r="B90" s="1">
         <v>0.24</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90" s="3">
         <v>0.21</v>
       </c>
       <c r="D90" s="1">
@@ -22666,7 +22659,7 @@
       <c r="B91" s="1">
         <v>0.25</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C91" s="3">
         <v>0.22</v>
       </c>
       <c r="D91" s="1">
@@ -22681,7 +22674,7 @@
       <c r="B92" s="1">
         <v>0.24</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C92" s="3">
         <v>0.21</v>
       </c>
       <c r="D92" s="1">
@@ -22696,7 +22689,7 @@
       <c r="B93" s="1">
         <v>0.25</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93" s="3">
         <v>0.21</v>
       </c>
       <c r="D93" s="1">
@@ -22711,7 +22704,7 @@
       <c r="B94" s="1">
         <v>0.24</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C94" s="3">
         <v>0.21</v>
       </c>
       <c r="D94" s="1">
@@ -22726,7 +22719,7 @@
       <c r="B95" s="1">
         <v>0.25</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C95" s="3">
         <v>0.21</v>
       </c>
       <c r="D95" s="1"/>
@@ -22739,7 +22732,7 @@
       <c r="B96" s="1">
         <v>0.24</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C96" s="3">
         <v>0.2</v>
       </c>
       <c r="D96" s="1"/>
@@ -22752,7 +22745,7 @@
       <c r="B97" s="1">
         <v>0.25</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C97" s="3">
         <v>0.21</v>
       </c>
       <c r="D97" s="1"/>
@@ -22765,7 +22758,7 @@
       <c r="B98" s="1">
         <v>0.24</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C98" s="3">
         <v>0.2</v>
       </c>
       <c r="D98" s="1"/>
@@ -22778,7 +22771,7 @@
       <c r="B99" s="1">
         <v>0.25</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C99" s="3">
         <v>0.2</v>
       </c>
       <c r="D99" s="1"/>
@@ -22791,7 +22784,7 @@
       <c r="B100" s="1">
         <v>0.24</v>
       </c>
-      <c r="C100" s="2">
+      <c r="C100" s="3">
         <v>0.2</v>
       </c>
       <c r="D100" s="1"/>
@@ -22804,7 +22797,7 @@
       <c r="B101" s="1">
         <v>0.25</v>
       </c>
-      <c r="C101" s="2">
+      <c r="C101" s="3">
         <v>0.2</v>
       </c>
       <c r="D101" s="1"/>
@@ -22817,7 +22810,7 @@
       <c r="B102" s="1">
         <v>0.24</v>
       </c>
-      <c r="C102" s="2">
+      <c r="C102" s="3">
         <v>0.19</v>
       </c>
       <c r="D102" s="1"/>
@@ -22830,7 +22823,7 @@
       <c r="B103" s="1">
         <v>0.25</v>
       </c>
-      <c r="C103" s="2">
+      <c r="C103" s="3">
         <v>0.19</v>
       </c>
       <c r="D103" s="1"/>
@@ -22843,7 +22836,7 @@
       <c r="B104" s="1">
         <v>0.24</v>
       </c>
-      <c r="C104" s="2">
+      <c r="C104" s="3">
         <v>0.19</v>
       </c>
       <c r="D104" s="1"/>
@@ -22856,7 +22849,7 @@
       <c r="B105" s="1">
         <v>0.25</v>
       </c>
-      <c r="C105" s="2">
+      <c r="C105" s="3">
         <v>0.19</v>
       </c>
       <c r="D105" s="1"/>
@@ -22869,7 +22862,7 @@
       <c r="B106" s="1">
         <v>0.24</v>
       </c>
-      <c r="C106" s="2">
+      <c r="C106" s="3">
         <v>0.18</v>
       </c>
       <c r="D106" s="1"/>
@@ -22882,7 +22875,7 @@
       <c r="B107" s="1">
         <v>0.25</v>
       </c>
-      <c r="C107" s="2">
+      <c r="C107" s="3">
         <v>0.19</v>
       </c>
       <c r="D107" s="1"/>
@@ -22895,7 +22888,7 @@
       <c r="B108" s="1">
         <v>0.24</v>
       </c>
-      <c r="C108" s="2">
+      <c r="C108" s="3">
         <v>0.17</v>
       </c>
       <c r="D108" s="1"/>
@@ -22908,7 +22901,7 @@
       <c r="B109" s="1">
         <v>0.25</v>
       </c>
-      <c r="C109" s="2">
+      <c r="C109" s="3">
         <v>0.18</v>
       </c>
       <c r="D109" s="1"/>
@@ -22921,7 +22914,7 @@
       <c r="B110" s="1">
         <v>0.24</v>
       </c>
-      <c r="C110" s="2">
+      <c r="C110" s="3">
         <v>0.17</v>
       </c>
       <c r="D110" s="1"/>
@@ -22934,7 +22927,7 @@
       <c r="B111" s="1">
         <v>0.25</v>
       </c>
-      <c r="C111" s="2">
+      <c r="C111" s="3">
         <v>0.17</v>
       </c>
       <c r="D111" s="1"/>
@@ -22947,7 +22940,7 @@
       <c r="B112" s="1">
         <v>0.24</v>
       </c>
-      <c r="C112" s="2">
+      <c r="C112" s="3">
         <v>0.16</v>
       </c>
       <c r="D112" s="1"/>
@@ -22960,7 +22953,7 @@
       <c r="B113" s="1">
         <v>0.25</v>
       </c>
-      <c r="C113" s="2">
+      <c r="C113" s="3">
         <v>0.16</v>
       </c>
       <c r="D113" s="1"/>
@@ -22973,7 +22966,7 @@
       <c r="B114" s="1">
         <v>0.24</v>
       </c>
-      <c r="C114" s="2">
+      <c r="C114" s="3">
         <v>0.15</v>
       </c>
       <c r="D114" s="1"/>
@@ -22986,7 +22979,7 @@
       <c r="B115" s="1">
         <v>0.25</v>
       </c>
-      <c r="C115" s="2">
+      <c r="C115" s="3">
         <v>0.15</v>
       </c>
       <c r="D115" s="1"/>
@@ -22999,7 +22992,7 @@
       <c r="B116" s="1">
         <v>0.24</v>
       </c>
-      <c r="C116" s="2">
+      <c r="C116" s="3">
         <v>0.15</v>
       </c>
       <c r="D116" s="1"/>
@@ -23012,7 +23005,7 @@
       <c r="B117" s="1">
         <v>0.25</v>
       </c>
-      <c r="C117" s="2">
+      <c r="C117" s="3">
         <v>0.15</v>
       </c>
       <c r="D117" s="1"/>
@@ -23025,7 +23018,7 @@
       <c r="B118" s="1">
         <v>0.24</v>
       </c>
-      <c r="C118" s="2">
+      <c r="C118" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D118" s="1"/>
@@ -23038,7 +23031,7 @@
       <c r="B119" s="1">
         <v>0.25</v>
       </c>
-      <c r="C119" s="2">
+      <c r="C119" s="3">
         <v>0.15</v>
       </c>
       <c r="D119" s="1"/>
@@ -23051,7 +23044,7 @@
       <c r="B120" s="1">
         <v>0.24</v>
       </c>
-      <c r="C120" s="2">
+      <c r="C120" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D120" s="1"/>
@@ -23064,7 +23057,7 @@
       <c r="B121" s="1">
         <v>0.25</v>
       </c>
-      <c r="C121" s="2">
+      <c r="C121" s="3">
         <v>0.15</v>
       </c>
       <c r="D121" s="1"/>
@@ -23077,7 +23070,7 @@
       <c r="B122" s="1">
         <v>0.24</v>
       </c>
-      <c r="C122" s="2">
+      <c r="C122" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D122" s="1"/>
@@ -23090,7 +23083,7 @@
       <c r="B123" s="1">
         <v>0.24</v>
       </c>
-      <c r="C123" s="2">
+      <c r="C123" s="3">
         <v>0.15</v>
       </c>
       <c r="D123" s="1"/>
@@ -23103,7 +23096,7 @@
       <c r="B124" s="1">
         <v>0.24</v>
       </c>
-      <c r="C124" s="2">
+      <c r="C124" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D124" s="1"/>
@@ -23116,7 +23109,7 @@
       <c r="B125" s="1">
         <v>0.24</v>
       </c>
-      <c r="C125" s="2">
+      <c r="C125" s="3">
         <v>0.15</v>
       </c>
       <c r="D125" s="1"/>
@@ -23129,7 +23122,7 @@
       <c r="B126" s="1">
         <v>0.24</v>
       </c>
-      <c r="C126" s="2">
+      <c r="C126" s="3">
         <v>0.13</v>
       </c>
       <c r="D126" s="1"/>
@@ -23142,7 +23135,7 @@
       <c r="B127" s="1">
         <v>0.24</v>
       </c>
-      <c r="C127" s="2">
+      <c r="C127" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D127" s="1"/>
@@ -23155,7 +23148,7 @@
       <c r="B128" s="1">
         <v>0.24</v>
       </c>
-      <c r="C128" s="2">
+      <c r="C128" s="3">
         <v>0.13</v>
       </c>
       <c r="D128" s="1"/>
@@ -23168,7 +23161,7 @@
       <c r="B129" s="1">
         <v>0.24</v>
       </c>
-      <c r="C129" s="2">
+      <c r="C129" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D129" s="1"/>
@@ -23181,7 +23174,7 @@
       <c r="B130" s="1">
         <v>0.24</v>
       </c>
-      <c r="C130" s="2">
+      <c r="C130" s="3">
         <v>0.13</v>
       </c>
       <c r="D130" s="1"/>
@@ -23194,7 +23187,7 @@
       <c r="B131" s="1">
         <v>0.24</v>
       </c>
-      <c r="C131" s="2">
+      <c r="C131" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D131" s="1"/>
@@ -23207,7 +23200,7 @@
       <c r="B132" s="1">
         <v>0.24</v>
       </c>
-      <c r="C132" s="2">
+      <c r="C132" s="3">
         <v>0.13</v>
       </c>
       <c r="D132" s="1"/>
@@ -23220,7 +23213,7 @@
       <c r="B133" s="1">
         <v>0.24</v>
       </c>
-      <c r="C133" s="2">
+      <c r="C133" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D133" s="1"/>
@@ -23233,7 +23226,7 @@
       <c r="B134" s="1">
         <v>0.24</v>
       </c>
-      <c r="C134" s="2">
+      <c r="C134" s="3">
         <v>0.13</v>
       </c>
       <c r="D134" s="1"/>
@@ -23246,7 +23239,7 @@
       <c r="B135" s="1">
         <v>0.24</v>
       </c>
-      <c r="C135" s="2">
+      <c r="C135" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D135" s="1"/>
@@ -23259,7 +23252,7 @@
       <c r="B136" s="1">
         <v>0.24</v>
       </c>
-      <c r="C136" s="2">
+      <c r="C136" s="3">
         <v>0.13</v>
       </c>
       <c r="D136" s="1"/>
@@ -23272,7 +23265,7 @@
       <c r="B137" s="1">
         <v>0.24</v>
       </c>
-      <c r="C137" s="2">
+      <c r="C137" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D137" s="1"/>
@@ -23285,7 +23278,7 @@
       <c r="B138" s="1">
         <v>0.24</v>
       </c>
-      <c r="C138" s="2">
+      <c r="C138" s="3">
         <v>0.13</v>
       </c>
       <c r="D138" s="1"/>
@@ -23298,7 +23291,7 @@
       <c r="B139" s="1">
         <v>0.24</v>
       </c>
-      <c r="C139" s="2">
+      <c r="C139" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D139" s="1"/>
@@ -23311,7 +23304,7 @@
       <c r="B140" s="1">
         <v>0.24</v>
       </c>
-      <c r="C140" s="2">
+      <c r="C140" s="3">
         <v>0.13</v>
       </c>
       <c r="D140" s="1"/>
@@ -23324,7 +23317,7 @@
       <c r="B141" s="1">
         <v>0.24</v>
       </c>
-      <c r="C141" s="2">
+      <c r="C141" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D141" s="1"/>
@@ -23337,7 +23330,7 @@
       <c r="B142" s="1">
         <v>0.24</v>
       </c>
-      <c r="C142" s="2">
+      <c r="C142" s="3">
         <v>0.13</v>
       </c>
       <c r="D142" s="1"/>
@@ -23350,7 +23343,7 @@
       <c r="B143" s="1">
         <v>0.24</v>
       </c>
-      <c r="C143" s="2">
+      <c r="C143" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D143" s="1"/>
@@ -23363,7 +23356,7 @@
       <c r="B144" s="1">
         <v>0.24</v>
       </c>
-      <c r="C144" s="2">
+      <c r="C144" s="3">
         <v>0.13</v>
       </c>
       <c r="D144" s="1"/>
@@ -23376,7 +23369,7 @@
       <c r="B145" s="1">
         <v>0.24</v>
       </c>
-      <c r="C145" s="2">
+      <c r="C145" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D145" s="1"/>
@@ -23389,7 +23382,7 @@
       <c r="B146" s="1">
         <v>0.24</v>
       </c>
-      <c r="C146" s="2">
+      <c r="C146" s="3">
         <v>0.13</v>
       </c>
       <c r="D146" s="1"/>
@@ -23402,7 +23395,7 @@
       <c r="B147" s="1">
         <v>0.24</v>
       </c>
-      <c r="C147" s="2">
+      <c r="C147" s="3">
         <v>0.13</v>
       </c>
       <c r="D147" s="1"/>
@@ -23415,7 +23408,7 @@
       <c r="B148" s="1">
         <v>0.24</v>
       </c>
-      <c r="C148" s="2">
+      <c r="C148" s="3">
         <v>0.13</v>
       </c>
       <c r="D148" s="1"/>
@@ -23428,7 +23421,7 @@
       <c r="B149" s="1">
         <v>0.24</v>
       </c>
-      <c r="C149" s="2">
+      <c r="C149" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D149" s="1"/>
@@ -23441,7 +23434,7 @@
       <c r="B150" s="1">
         <v>0.24</v>
       </c>
-      <c r="C150" s="2">
+      <c r="C150" s="3">
         <v>0.12</v>
       </c>
       <c r="D150" s="1"/>
@@ -23454,7 +23447,7 @@
       <c r="B151" s="1">
         <v>0.24</v>
       </c>
-      <c r="C151" s="2">
+      <c r="C151" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D151" s="1"/>
@@ -23467,7 +23460,7 @@
       <c r="B152" s="1">
         <v>0.24</v>
       </c>
-      <c r="C152" s="2">
+      <c r="C152" s="3">
         <v>0.13</v>
       </c>
       <c r="D152" s="1"/>
@@ -23480,7 +23473,7 @@
       <c r="B153" s="1">
         <v>0.24</v>
       </c>
-      <c r="C153" s="2">
+      <c r="C153" s="3">
         <v>0.13</v>
       </c>
       <c r="D153" s="1"/>
@@ -23493,7 +23486,7 @@
       <c r="B154" s="1">
         <v>0.24</v>
       </c>
-      <c r="C154" s="2">
+      <c r="C154" s="3">
         <v>0.12</v>
       </c>
       <c r="D154" s="1"/>
@@ -23506,7 +23499,7 @@
       <c r="B155" s="1">
         <v>0.24</v>
       </c>
-      <c r="C155" s="2">
+      <c r="C155" s="3">
         <v>0.13</v>
       </c>
       <c r="D155" s="1"/>
@@ -23519,7 +23512,7 @@
       <c r="B156" s="1">
         <v>0.24</v>
       </c>
-      <c r="C156" s="2">
+      <c r="C156" s="3">
         <v>0.12</v>
       </c>
       <c r="D156" s="1"/>
@@ -23532,7 +23525,7 @@
       <c r="B157" s="1">
         <v>0.24</v>
       </c>
-      <c r="C157" s="2">
+      <c r="C157" s="3">
         <v>0.13</v>
       </c>
       <c r="D157" s="1"/>
@@ -23545,7 +23538,7 @@
       <c r="B158" s="1">
         <v>0.24</v>
       </c>
-      <c r="C158" s="2">
+      <c r="C158" s="3">
         <v>0.12</v>
       </c>
       <c r="D158" s="1"/>
@@ -23558,7 +23551,7 @@
       <c r="B159" s="1">
         <v>0.24</v>
       </c>
-      <c r="C159" s="2">
+      <c r="C159" s="3">
         <v>0.13</v>
       </c>
       <c r="D159" s="1"/>
@@ -23571,7 +23564,7 @@
       <c r="B160" s="1">
         <v>0.24</v>
       </c>
-      <c r="C160" s="2">
+      <c r="C160" s="3">
         <v>0.12</v>
       </c>
       <c r="D160" s="1"/>
@@ -23584,7 +23577,7 @@
       <c r="B161" s="1">
         <v>0.24</v>
       </c>
-      <c r="C161" s="2">
+      <c r="C161" s="3">
         <v>0.13</v>
       </c>
       <c r="D161" s="1"/>
@@ -23597,7 +23590,7 @@
       <c r="B162" s="1">
         <v>0.24</v>
       </c>
-      <c r="C162" s="2">
+      <c r="C162" s="3">
         <v>0.12</v>
       </c>
       <c r="D162" s="1"/>
@@ -23610,7 +23603,7 @@
       <c r="B163" s="1">
         <v>0.24</v>
       </c>
-      <c r="C163" s="2">
+      <c r="C163" s="3">
         <v>0.13</v>
       </c>
       <c r="D163" s="1"/>
@@ -23623,7 +23616,7 @@
       <c r="B164" s="1">
         <v>0.24</v>
       </c>
-      <c r="C164" s="2">
+      <c r="C164" s="3">
         <v>0.12</v>
       </c>
       <c r="D164" s="1"/>
@@ -23636,7 +23629,7 @@
       <c r="B165" s="1">
         <v>0.24</v>
       </c>
-      <c r="C165" s="2">
+      <c r="C165" s="3">
         <v>0.13</v>
       </c>
       <c r="D165" s="1"/>
@@ -23649,7 +23642,7 @@
       <c r="B166" s="1">
         <v>0.24</v>
       </c>
-      <c r="C166" s="2">
+      <c r="C166" s="3">
         <v>0.12</v>
       </c>
       <c r="D166" s="1"/>
@@ -23662,7 +23655,7 @@
       <c r="B167" s="1">
         <v>0.24</v>
       </c>
-      <c r="C167" s="2">
+      <c r="C167" s="3">
         <v>0.12</v>
       </c>
       <c r="D167" s="1"/>
@@ -23675,7 +23668,7 @@
       <c r="B168" s="1">
         <v>0.24</v>
       </c>
-      <c r="C168" s="2">
+      <c r="C168" s="3">
         <v>0.12</v>
       </c>
       <c r="D168" s="1"/>
@@ -23688,7 +23681,7 @@
       <c r="B169" s="1">
         <v>0.24</v>
       </c>
-      <c r="C169" s="2">
+      <c r="C169" s="3">
         <v>0.12</v>
       </c>
       <c r="D169" s="1"/>
@@ -23701,7 +23694,7 @@
       <c r="B170" s="1">
         <v>0.24</v>
       </c>
-      <c r="C170" s="2">
+      <c r="C170" s="3">
         <v>0.12</v>
       </c>
       <c r="D170" s="1"/>
@@ -23714,7 +23707,7 @@
       <c r="B171" s="1">
         <v>0.24</v>
       </c>
-      <c r="C171" s="2">
+      <c r="C171" s="3">
         <v>0.11</v>
       </c>
       <c r="D171" s="1"/>
@@ -23727,7 +23720,7 @@
       <c r="B172" s="1">
         <v>0.24</v>
       </c>
-      <c r="C172" s="2">
+      <c r="C172" s="3">
         <v>0.11</v>
       </c>
       <c r="D172" s="1"/>
@@ -23740,7 +23733,7 @@
       <c r="B173" s="1">
         <v>0.24</v>
       </c>
-      <c r="C173" s="2">
+      <c r="C173" s="3">
         <v>0.11</v>
       </c>
       <c r="D173" s="1"/>
@@ -23753,7 +23746,7 @@
       <c r="B174" s="1">
         <v>0.24</v>
       </c>
-      <c r="C174" s="2">
+      <c r="C174" s="3">
         <v>0.1</v>
       </c>
       <c r="D174" s="1"/>
@@ -23766,7 +23759,7 @@
       <c r="B175" s="1">
         <v>0.24</v>
       </c>
-      <c r="C175" s="2">
+      <c r="C175" s="3">
         <v>0.11</v>
       </c>
       <c r="D175" s="1"/>
@@ -23779,7 +23772,7 @@
       <c r="B176" s="1">
         <v>0.24</v>
       </c>
-      <c r="C176" s="2">
+      <c r="C176" s="3">
         <v>0.11</v>
       </c>
       <c r="D176" s="1"/>
@@ -23792,7 +23785,7 @@
       <c r="B177" s="1">
         <v>0.24</v>
       </c>
-      <c r="C177" s="2">
+      <c r="C177" s="3">
         <v>0.11</v>
       </c>
       <c r="D177" s="1"/>
@@ -23805,7 +23798,7 @@
       <c r="B178" s="1">
         <v>0.24</v>
       </c>
-      <c r="C178" s="2">
+      <c r="C178" s="3">
         <v>0.11</v>
       </c>
       <c r="D178" s="1"/>
@@ -23818,7 +23811,7 @@
       <c r="B179" s="1">
         <v>0.23</v>
       </c>
-      <c r="C179" s="2">
+      <c r="C179" s="3">
         <v>0.11</v>
       </c>
       <c r="D179" s="1"/>
@@ -23831,7 +23824,7 @@
       <c r="B180" s="1">
         <v>0.24</v>
       </c>
-      <c r="C180" s="2">
+      <c r="C180" s="3">
         <v>0.1</v>
       </c>
       <c r="D180" s="1"/>
@@ -23844,7 +23837,7 @@
       <c r="B181" s="1">
         <v>0.23</v>
       </c>
-      <c r="C181" s="2">
+      <c r="C181" s="3">
         <v>0.11</v>
       </c>
       <c r="D181" s="1"/>
@@ -23857,7 +23850,7 @@
       <c r="B182" s="1">
         <v>0.24</v>
       </c>
-      <c r="C182" s="2">
+      <c r="C182" s="3">
         <v>0.11</v>
       </c>
       <c r="D182" s="1"/>
@@ -23870,7 +23863,7 @@
       <c r="B183" s="1">
         <v>0.23</v>
       </c>
-      <c r="C183" s="2">
+      <c r="C183" s="3">
         <v>0.11</v>
       </c>
       <c r="D183" s="1"/>
@@ -23883,7 +23876,7 @@
       <c r="B184" s="1">
         <v>0.24</v>
       </c>
-      <c r="C184" s="2">
+      <c r="C184" s="3">
         <v>0.11</v>
       </c>
       <c r="D184" s="1"/>
@@ -23896,7 +23889,7 @@
       <c r="B185" s="1">
         <v>0.23</v>
       </c>
-      <c r="C185" s="2">
+      <c r="C185" s="3">
         <v>0.11</v>
       </c>
       <c r="D185" s="1"/>
@@ -23909,7 +23902,7 @@
       <c r="B186" s="1">
         <v>0.24</v>
       </c>
-      <c r="C186" s="1"/>
+      <c r="C186" s="3"/>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
     </row>
@@ -23920,7 +23913,7 @@
       <c r="B187" s="1">
         <v>0.23</v>
       </c>
-      <c r="C187" s="1"/>
+      <c r="C187" s="3"/>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
     </row>
@@ -23931,7 +23924,7 @@
       <c r="B188" s="1">
         <v>0.24</v>
       </c>
-      <c r="C188" s="1"/>
+      <c r="C188" s="3"/>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
     </row>
@@ -23942,7 +23935,7 @@
       <c r="B189" s="1">
         <v>0.23</v>
       </c>
-      <c r="C189" s="1"/>
+      <c r="C189" s="3"/>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
     </row>
@@ -23953,7 +23946,7 @@
       <c r="B190" s="1">
         <v>0.23</v>
       </c>
-      <c r="C190" s="1"/>
+      <c r="C190" s="3"/>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
     </row>
@@ -23964,7 +23957,7 @@
       <c r="B191" s="1">
         <v>0.23</v>
       </c>
-      <c r="C191" s="1"/>
+      <c r="C191" s="3"/>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
     </row>
@@ -23975,7 +23968,7 @@
       <c r="B192" s="1">
         <v>0.23</v>
       </c>
-      <c r="C192" s="1"/>
+      <c r="C192" s="3"/>
       <c r="D192" s="1"/>
       <c r="E192" s="1"/>
     </row>
@@ -23986,7 +23979,7 @@
       <c r="B193" s="1">
         <v>0.23</v>
       </c>
-      <c r="C193" s="1"/>
+      <c r="C193" s="3"/>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
     </row>
@@ -23997,7 +23990,7 @@
       <c r="B194" s="1">
         <v>0.23</v>
       </c>
-      <c r="C194" s="1"/>
+      <c r="C194" s="3"/>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
     </row>
@@ -24008,7 +24001,7 @@
       <c r="B195" s="1">
         <v>0.23</v>
       </c>
-      <c r="C195" s="1"/>
+      <c r="C195" s="3"/>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
     </row>
@@ -24019,7 +24012,7 @@
       <c r="B196" s="1">
         <v>0.23</v>
       </c>
-      <c r="C196" s="1"/>
+      <c r="C196" s="3"/>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
     </row>
@@ -24030,7 +24023,7 @@
       <c r="B197" s="1">
         <v>0.23</v>
       </c>
-      <c r="C197" s="1"/>
+      <c r="C197" s="3"/>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
     </row>
@@ -24041,7 +24034,7 @@
       <c r="B198" s="1">
         <v>0.23</v>
       </c>
-      <c r="C198" s="1"/>
+      <c r="C198" s="3"/>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
     </row>
@@ -24052,7 +24045,7 @@
       <c r="B199" s="1">
         <v>0.23</v>
       </c>
-      <c r="C199" s="1"/>
+      <c r="C199" s="3"/>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
     </row>
@@ -24063,7 +24056,7 @@
       <c r="B200" s="1">
         <v>0.23</v>
       </c>
-      <c r="C200" s="1"/>
+      <c r="C200" s="3"/>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
     </row>
@@ -24074,7 +24067,7 @@
       <c r="B201" s="1">
         <v>0.23</v>
       </c>
-      <c r="C201" s="1"/>
+      <c r="C201" s="3"/>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
     </row>
@@ -24083,7 +24076,7 @@
         <v>10000</v>
       </c>
       <c r="B202" s="1"/>
-      <c r="C202" s="1"/>
+      <c r="C202" s="3"/>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
     </row>
@@ -27151,7 +27144,7 @@
   <dimension ref="A1:G202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G38"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>